<commit_message>
Crosswalks updated to NACC 20250626
</commit_message>
<xml_diff>
--- a/Crosswalk/A1_UDS4_programmatic_crosswalk.xlsx
+++ b/Crosswalk/A1_UDS4_programmatic_crosswalk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfmurch\Desktop\Json_SOPS\Crosswalk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UAB Neurology\NACC and UDS\Json_SOPS\Crosswalk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8555" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8555" uniqueCount="1141">
   <si>
     <t>TEMPLATE - UDS3 DED (Data Element Dictionary) and RDD (Researcher's Data Dictionary)
 Based on Data Element and Researcher's Data Dictionary PDF at https://naccdata.org/data-collection/forms-documentation/uds-3</t>
@@ -4410,9 +4410,6 @@
     <t>100 | 101 | 102 | 103 | 104 | 105 | 106 | 107 | 108 | 109 | 110 | 111 | 112 | 113 | 114 | 115 | 116 | 117 | 118 | 119 | 120 | 121 | 122 | 123 | 124 | 200 | 201 | 202 | 203 | 204 | 205 | 206 | 207 | 208 | 209 | 210 | 211 | 212 | 213 | 214 | 215 | 216 | 217 | 218 | 219 | 220 | 221 | 222 | 223 | 224 | 225 | 226 | 227 | 228 | 229 | 230 | 231 | 232 | 233 | 234 | 235 | 236 | 237 | 238 | 239 | 240 | 300 | 301 | 302 | 303 | 304 | 305 | 306 | 307 | 308 | 309 | 310 | 311 | 312 | 313 | 314 | 315 | 316 | 317 | 318 | 319 | 320 | 321 | 322 | 323 | 324 | 325 | 326 | 327 | 328 | 329 | 330 | 331 | 332 | 333 | 334 | 335 | 336 | 337 | 338 | 339 | 400 | 401 | 402 | 403 | 404 | 405 | 406 | 407 | 408 | 409 | 410 | 411 | 412 | 413 | 414 | 415 | 416 | 417 | 418 | 419 | 420 | 421 | 422 | 423 | 424 | 425 | 426 | 427 | 428 | 429 | 430 | 431 | 432 | 500 | 501 | 502 | 503 | 504 | 505 | 506 | 507 | 508 | 509 | 510 | 511 | 512 | 513 | 514 | 515 | 516 | 517 | 518 | 519 | 520 | 521 | 522 | 523 | 524 | 525 | 526 | 527 | 528 | 529 | 530 | 531 | 532 | 533 | 534 | 535 | 536 | 537 | 538 | 539 | 540 | 541 | 542 | 543 | 544 | 545 | 546 | 547 | 548 | 549 | 550 | 551 | 552 | 553 | 554 | 555 | 556 | 600 | 601 | 602 | 603 | 604 | 605 | 606 | 607 | 608 | 609 | 610 | 611 | 612 | 613 | 614 | 615 | 616 | 617 | 618 | 619 | 620 | 621 | 622 | 623 | 624 | 625 | 626 | 627 | 628 | 629 | 630 | 631 | 632 | 633 | 700 | 701 | 702 | 703 | 704 | 705 | 706 | 707 | 708 | 709 | 710 | 711 | 712 | 713 | 714 | 715 | 716 | 717 | 718 | 719 | 720 | 721 | 722 | 723 | 724 | 725 | 726 | 727 | 728 | 729 | 730 | 731</t>
   </si>
   <si>
-    <t>100 - Major professionals/ Higher Executives/ Proprietors of Large Concerns | 101 - Actuaries | 102 - Architects | 103 - Bank officers | 104 - Certified public accountants | 105 - Chief executives (CEO | 106 - Clergy (professionally trained) | 107 - Commissioned officers in the military | 108 - Dentists | 109 - Economists | 110 - Engineers (Masters level and above) | 111 - Financial managers | 112 - Federal government officials | 113 - Large business owners | 114 - Lawyers / judges | 115 - Mathematicians | 116 - Major contractors | 117 - Orthodontists | 118 - Physicians | 119 - Professor / University teachers | 120 - Psychologists | 121 - Research scientists | 122 - Urban and regional planners | 123 - Veterinarians | 124 - VP of large business | 200 - Lesser Professionals/ Business Managers of Medium-sized Businesses | 201 - Accountants | 202 - Advertising executives | 203 - Authors | 204 - Branch managers | 205 - Building contractors | 206 - Business managers | 207 - Chiropractors | 208 - Computer programmer | 209 - Computer specialists | 210 - Database developer | 211 - Editors | 212 - Engineers (no advanced degree) | 213 - Executive managers | 214 - Industrial farm owners | 215 - Furniture business owners | 216 - Jewelers | 217 - Labor relations consultant | 218 - Librarians | 219 - Manufacturing owners | 220 - Medium business owners | 221 - Musicians / composers | 222 - Nurses | 223 - Office managers | 224 - Opticians | 225 - Personnel managers | 226 - Pharmacists | 227 - Pilots | 228 - Police chief / sheriff | 229 - Postmaster | 230 - Production managers (TV / Radio) | 231 - Public administration officials | 232 - Public health officers | 233 - Purchasing managers | 234 - Real estate brokers | 235 - Research assistants | 236 - Sales engineers | 237 - Sales managers | 238 - Social workers | 239 - State / Local government officials | 240 - Teachers (Elementary &amp; high school) | 300 - Administrative Personnel/Small Business Owners/ Minor Professionals | 301 - Actors | 302 - Administrative assistants | 303 - Advertising agents | 304 - Artists | 305 - Bakers | 306 - Beauty shop owners | 307 - Chefs | 308 - Chief clerks | 309 - Clergy (not professionally trained) | 310 - Court reporters | 311 - Credit managers | 312 - Dental hygienists | 313 - Department store managers | 314 - Deputy sheriffs | 315 - Dietitians / Nutritionists | 316 - Dispatchers | 317 - Florists | 318 - Funeral directors | 319 - Insurance agents | 320 - Laboratory assistants | 321 - Landscape planners | 322 - Noncommissioned officers in the military (at or above rank of master sergeant / C.P.O.) | 323 - Morticians | 324 - Newspaper / TV reporters | 325 - Photographers | 326 - Piano teachers | 327 - Radio / TV announcers | 328 - Real estate agents | 329 - Restaurant owners | 330 - Sales representatives | 331 - Service managers | 332 - Small business owners | 333 - Store managers | 334 - Surveyors | 335 - Title searchers | 336 - Tool designers | 337 - Traffic managers | 338 - Travel agents | 339 - Yard masters (Railroad) | 400 - Clerical and Sales Workers/Technicians/ Owners of Little Businesses | 401 - Bank tellers | 402 - Bill collectors | 403 - Bookkeepers | 404 - Claims examiners | 405 - Drafters | 406 - Driving teachers | 407 - Factory supervisors | 408 - Small farm owners / farmers | 409 - Flower shop workers | 410 - Human resources workers | 411 - Laboratory technicians | 412 - Newsstand operators | 413 - Post office clerks | 414 - Railroad conductors | 415 - Railroad train engineers | 416 - Receptionists | 417 - Route managers | 418 - Sales clerks | 419 - Secretaries / stenographers | 420 - Shipping clerks | 421 - Tailors | 422 - Tax clerks | 423 - Telephone company workers | 424 - Telephone operators | 425 - Timekeepers | 426 - Toll collectors | 427 - Tower operators | 428 - Truck dispatchers | 429 - Typists | 430 - Utility workers | 431 - Warehouse clerks | 432 - Window store trimmers | 500 - Skilled Manual Employees | 501 - Auto body repairers | 502 - Barbers | 503 - Boiler repairers | 504 - Bookbinders | 505 - Brewers | 506 - Cabinet makers | 507 - Carpenters | 508 - Cement layers / finishers | 509 - Checkers / examiners / inspectors | 510 - Cheese makers | 511 - Construction forepeople | 512 - Die makers | 513 - Electricians | 514 - Engravers | 515 - Exterminators | 516 - Firefighters | 517 - Gardeners / landscapers | 518 - Glassblowers | 519 - Glaziers | 520 - Gun smiths | 521 - Hair stylists | 522 - Heavy equipment operators | 523 - Home repairs | 524 - Iron workers | 525 - Kitchen workers / cooks | 526 - Locksmiths | 527 - Machinists | 528 - Mail carriers | 529 - Maintenance forepeople | 530 - Masons | 531 - Mechanics | 532 - Millwrights | 533 - Noncommissioned officers in the military (below rank of master sergeant / C.P.O.) | 534 - Painters | 535 - Paperhangers | 536 - Patrolmen | 537 - Piano builders | 538 - Piano tuners | 539 - Plumbers | 540 - Police officers | 541 - Postal workers | 542 - Printers | 543 - Radio / TV maintenance | 544 - Railroad brake operators | 545 - Repair people | 546 - Seamstresses / seamsters | 547 - Sheet metal workers | 548 - Ship smiths | 549 - Shoe repairers | 550 - Steelworkers | 551 - Tile layers | 552 - Tool makers | 553 - Upholsterers | 554 - Utility line workers | 555 - Weavers | 556 - Welders | 600 - Machine Operators/ Semiskilled Employees | 601 - Apprentices (electrician / printers / etc.) | 602 - Assembly line workers | 603 - Bartenders | 604 - Building superintendents | 605 - Bus drivers | 606 - Cab / taxi drivers | 607 - Cashiers | 608 - Child care workers (not private household) | 609 - Cooks (short order) | 610 - Corrections workers | 611 - Delivery people | 612 - Dry cleaning pressers | 613 - Elevator operators | 614 - Enlisted military personnel (other than noncommissioned officers) | 615 - Factory machine operators | 616 - Factory workers | 617 - Foundry workers | 618 - Garage and gas station assistants | 619 - Greenhouse workers | 620 - Guards / security watch people | 621 - Machine operators | 622 - Meat cutters / packers | 623 - Meter readers | 624 - Nursing aides / attendants | 625 - Oil delivery people | 626 - Practical nurses | 627 - Pump operators | 628 - Receivers / checkers | 629 - Servers (waiters / waitresses) | 630 - Signal operators (railroad) | 631 - Truck drivers | 632 - Wood workers | 633 - Wrappers (stores / factories) | 700 - Unskilled Employees | 701 - Amusement park workers | 702 - Cafeteria workers | 703 - Car cleaners | 704 - Child care workers (private household) | 705 - Construction laborers | 706 - Dairy workers | 707 - Deck hands | 708 - Farm laborers | 709 - Fishers | 710 - Freight handlers | 711 - Garbage collectors | 712 - Grave diggers | 713 - Homemakers | 714 - House cleaners | 715 - Janitors | 716 - Junk / recycle sorters | 717 - Laundry workers | 718 - Messengers | 719 - Peddlers | 720 - Porters | 721 - Roofing laborers | 722 - Shoe shiners | 723 - Stagehands | 724 - Stock handlers | 725 - Street cleaners | 726 - Unemployed | 727 - Unskilled factory workers | 728 - Unspecified laborers | 729 - Window cleaners | 730 - Woodchoppers | 731 - Worked while incarcerated</t>
-  </si>
-  <si>
     <t>1-4</t>
   </si>
   <si>
@@ -4552,6 +4549,15 @@
   </si>
   <si>
     <t>Website</t>
+  </si>
+  <si>
+    <t>100 - Major professionals/ Higher Executives/ Proprietors of Large Concerns | 101 - Actuaries | 102 - Architects | 103 - Bank officers | 104 - Certified public accountants | 105 - Chief executives (CEO, CFO, COO) | 106 - Clergy (professionally trained) | 107 - Commissioned officers in the military | 108 - Dentists | 109 - Economists | 110 - Engineers (Masters level and above) | 111 - Financial managers | 112 - Federal government officials | 113 - Large business owners | 114 - Lawyers / judges | 115 - Mathematicians | 116 - Major contractors | 117 - Orthodontists | 118 - Physicians | 119 - Professor / University teachers | 120 - Psychologists | 121 - Research scientists | 122 - Urban and regional planners | 123 - Veterinarians | 124 - VP of large business | 200 - Lesser Professionals/ Business Managers of Medium-sized Businesses | 201 - Accountants | 202 - Advertising executives | 203 - Authors | 204 - Branch managers | 205 - Building contractors | 206 - Business managers | 207 - Chiropractors | 208 - Computer programmer | 209 - Computer specialists | 210 - Database developer | 211 - Editors | 212 - Engineers (no advanced degree) | 213 - Executive managers | 214 - Industrial farm owners | 215 - Furniture business owners | 216 - Jewelers | 217 - Labor relations consultant | 218 - Librarians | 219 - Manufacturing owners | 220 - Medium business owners | 221 - Musicians / composers | 222 - Nurses | 223 - Office managers | 224 - Opticians | 225 - Personnel managers | 226 - Pharmacists | 227 - Pilots | 228 - Police chief / sheriff | 229 - Postmaster | 230 - Production managers (TV / Radio) | 231 - Public administration officials | 232 - Public health officers | 233 - Purchasing managers | 234 - Real estate brokers | 235 - Research assistants | 236 - Sales engineers | 237 - Sales managers | 238 - Social workers | 239 - State / Local government officials | 240 - Teachers (Elementary &amp; high school) | 300 - Administrative Personnel/Small Business Owners/ Minor Professionals | 301 - Actors | 302 - Administrative assistants | 303 - Advertising agents | 304 - Artists | 305 - Bakers | 306 - Beauty shop owners | 307 - Chefs | 308 - Chief clerks | 309 - Clergy (not professionally trained) | 310 - Court reporters | 311 - Credit managers | 312 - Dental hygienists | 313 - Department store managers | 314 - Deputy sheriffs | 315 - Dietitians / Nutritionists | 316 - Dispatchers | 317 - Florists | 318 - Funeral directors | 319 - Insurance agents | 320 - Laboratory assistants | 321 - Landscape planners | 322 - Noncommissioned officers in the military (at or above rank of master sergeant / C.P.O.) | 323 - Morticians | 324 - Newspaper / TV reporters | 325 - Photographers | 326 - Piano teachers | 327 - Radio / TV announcers | 328 - Real estate agents | 329 - Restaurant owners | 330 - Sales representatives | 331 - Service managers | 332 - Small business owners | 333 - Store managers | 334 - Surveyors | 335 - Title searchers | 336 - Tool designers | 337 - Traffic managers | 338 - Travel agents | 339 - Yard masters (Railroad) | 400 - Clerical and Sales Workers/Technicians/ Owners of Little Businesses | 401 - Bank tellers | 402 - Bill collectors | 403 - Bookkeepers | 404 - Claims examiners | 405 - Drafters | 406 - Driving teachers | 407 - Factory supervisors | 408 - Small farm owners / farmers | 409 - Flower shop workers | 410 - Human resources workers | 411 - Laboratory technicians | 412 - Newsstand operators | 413 - Post office clerks | 414 - Railroad conductors | 415 - Railroad train engineers | 416 - Receptionists | 417 - Route managers | 418 - Sales clerks | 419 - Secretaries / stenographers | 420 - Shipping clerks | 421 - Tailors | 422 - Tax clerks | 423 - Telephone company workers | 424 - Telephone operators | 425 - Timekeepers | 426 - Toll collectors | 427 - Tower operators | 428 - Truck dispatchers | 429 - Typists | 430 - Utility workers | 431 - Warehouse clerks | 432 - Window store trimmers | 500 - Skilled Manual Employees | 501 - Auto body repairers | 502 - Barbers | 503 - Boiler repairers | 504 - Bookbinders | 505 - Brewers | 506 - Cabinet makers | 507 - Carpenters | 508 - Cement layers / finishers | 509 - Checkers / examiners / inspectors | 510 - Cheese makers | 511 - Construction forepeople | 512 - Die makers | 513 - Electricians | 514 - Engravers | 515 - Exterminators | 516 - Firefighters | 517 - Gardeners / landscapers | 518 - Glassblowers | 519 - Glaziers | 520 - Gun smiths | 521 - Hair stylists | 522 - Heavy equipment operators | 523 - Home repairs | 524 - Iron workers | 525 - Kitchen workers / cooks | 526 - Locksmiths | 527 - Machinists | 528 - Mail carriers | 529 - Maintenance forepeople | 530 - Masons | 531 - Mechanics | 532 - Millwrights | 533 - Noncommissioned officers in the military (below rank of master sergeant / C.P.O.) | 534 - Painters | 535 - Paperhangers | 536 - Patrolmen | 537 - Piano builders | 538 - Piano tuners | 539 - Plumbers | 540 - Police officers | 541 - Postal workers | 542 - Printers | 543 - Radio / TV maintenance | 544 - Railroad brake operators | 545 - Repair people | 546 - Seamstresses / seamsters | 547 - Sheet metal workers | 548 - Ship smiths | 549 - Shoe repairers | 550 - Steelworkers | 551 - Tile layers | 552 - Tool makers | 553 - Upholsterers | 554 - Utility line workers | 555 - Weavers | 556 - Welders | 600 - Machine Operators/ Semiskilled Employees | 601 - Apprentices (electrician / printers / etc.) | 602 - Assembly line workers | 603 - Bartenders | 604 - Building superintendents | 605 - Bus drivers | 606 - Cab / taxi drivers | 607 - Cashiers | 608 - Child care workers (not private household) | 609 - Cooks (short order) | 610 - Corrections workers | 611 - Delivery people | 612 - Dry cleaning pressers | 613 - Elevator operators | 614 - Enlisted military personnel (other than noncommissioned officers) | 615 - Factory machine operators | 616 - Factory workers | 617 - Foundry workers | 618 - Garage and gas station assistants | 619 - Greenhouse workers | 620 - Guards / security watch people | 621 - Machine operators | 622 - Meat cutters / packers | 623 - Meter readers | 624 - Nursing aides / attendants | 625 - Oil delivery people | 626 - Practical nurses | 627 - Pump operators | 628 - Receivers / checkers | 629 - Servers (waiters / waitresses) | 630 - Signal operators (railroad) | 631 - Truck drivers | 632 - Wood workers | 633 - Wrappers (stores / factories) | 700 - Unskilled Employees | 701 - Amusement park workers | 702 - Cafeteria workers | 703 - Car cleaners | 704 - Child care workers (private household) | 705 - Construction laborers | 706 - Dairy workers | 707 - Deck hands | 708 - Farm laborers | 709 - Fishers | 710 - Freight handlers | 711 - Garbage collectors | 712 - Grave diggers | 713 - Homemakers | 714 - House cleaners | 715 - Janitors | 716 - Junk / recycle sorters | 717 - Laundry workers | 718 - Messengers | 719 - Peddlers | 720 - Porters | 721 - Roofing laborers | 722 - Shoe shiners | 723 - Stagehands | 724 - Stock handlers | 725 - Street cleaners | 726 - Unemployed | 727 - Unskilled factory workers | 728 - Unspecified laborers | 729 - Window cleaners | 730 - Woodchoppers | 731 - Worked while incarcerated</t>
+  </si>
+  <si>
+    <t>1 | 2 | 3 | 4 | 6 | 9</t>
+  </si>
+  <si>
+    <t>1-4, 6, 9</t>
   </si>
 </sst>
 </file>
@@ -5048,13 +5054,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -5448,21 +5454,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.5" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="E1" s="55" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="E1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="I1" s="55" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="I1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -5494,7 +5500,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -5504,7 +5510,7 @@
         <v>1041</v>
       </c>
       <c r="D3" s="17"/>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="55" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="28" t="s">
@@ -5514,7 +5520,7 @@
         <v>1042</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="55" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="28" t="s">
@@ -5525,7 +5531,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="117.75" customHeight="1" thickBot="1">
-      <c r="A4" s="53"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="29" t="s">
         <v>9</v>
       </c>
@@ -5533,7 +5539,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="17"/>
-      <c r="E4" s="53"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="29" t="s">
         <v>9</v>
       </c>
@@ -5541,7 +5547,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="17"/>
-      <c r="I4" s="53"/>
+      <c r="I4" s="55"/>
       <c r="J4" s="29" t="s">
         <v>11</v>
       </c>
@@ -5550,7 +5556,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="55" t="s">
         <v>1044</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -5560,7 +5566,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="55" t="s">
         <v>1044</v>
       </c>
       <c r="F5" s="28" t="s">
@@ -5570,7 +5576,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="55" t="s">
         <v>1044</v>
       </c>
       <c r="J5" s="28" t="s">
@@ -5581,7 +5587,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="45.75" thickBot="1">
-      <c r="A6" s="53"/>
+      <c r="A6" s="55"/>
       <c r="B6" s="31" t="s">
         <v>17</v>
       </c>
@@ -5589,7 +5595,7 @@
         <v>1045</v>
       </c>
       <c r="D6" s="17"/>
-      <c r="E6" s="53"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="31" t="s">
         <v>17</v>
       </c>
@@ -5597,7 +5603,7 @@
         <v>1045</v>
       </c>
       <c r="H6" s="17"/>
-      <c r="I6" s="53"/>
+      <c r="I6" s="55"/>
       <c r="J6" s="31" t="s">
         <v>18</v>
       </c>
@@ -5606,7 +5612,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A7" s="53"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
@@ -5614,7 +5620,7 @@
         <v>1047</v>
       </c>
       <c r="D7" s="17"/>
-      <c r="E7" s="53"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="33" t="s">
         <v>19</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>1048</v>
       </c>
       <c r="H7" s="17"/>
-      <c r="I7" s="53"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="33" t="s">
         <v>19</v>
       </c>
@@ -5631,7 +5637,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A8" s="53"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="31" t="s">
         <v>20</v>
       </c>
@@ -5639,7 +5645,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="53"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="31" t="s">
         <v>20</v>
       </c>
@@ -5647,7 +5653,7 @@
         <v>22</v>
       </c>
       <c r="H8" s="17"/>
-      <c r="I8" s="53"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="31" t="s">
         <v>20</v>
       </c>
@@ -5656,7 +5662,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A9" s="53"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="33" t="s">
         <v>24</v>
       </c>
@@ -5664,7 +5670,7 @@
         <v>1049</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="53"/>
+      <c r="E9" s="55"/>
       <c r="F9" s="33" t="s">
         <v>24</v>
       </c>
@@ -5672,7 +5678,7 @@
         <v>1050</v>
       </c>
       <c r="H9" s="17"/>
-      <c r="I9" s="53"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="33" t="s">
         <v>24</v>
       </c>
@@ -5681,7 +5687,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A10" s="53"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="31" t="s">
         <v>25</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="53"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="31" t="s">
         <v>25</v>
       </c>
@@ -5697,7 +5703,7 @@
         <v>1051</v>
       </c>
       <c r="H10" s="17"/>
-      <c r="I10" s="53"/>
+      <c r="I10" s="55"/>
       <c r="J10" s="31" t="s">
         <v>25</v>
       </c>
@@ -5706,7 +5712,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A11" s="53"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
@@ -5714,7 +5720,7 @@
         <v>28</v>
       </c>
       <c r="D11" s="17"/>
-      <c r="E11" s="53"/>
+      <c r="E11" s="55"/>
       <c r="F11" s="33" t="s">
         <v>27</v>
       </c>
@@ -5722,7 +5728,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="53"/>
+      <c r="I11" s="55"/>
       <c r="J11" s="33" t="s">
         <v>27</v>
       </c>
@@ -5731,7 +5737,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A12" s="53"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="31" t="s">
         <v>1052</v>
       </c>
@@ -5739,7 +5745,7 @@
         <v>1053</v>
       </c>
       <c r="D12" s="17"/>
-      <c r="E12" s="53"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="31" t="s">
         <v>1052</v>
       </c>
@@ -5747,7 +5753,7 @@
         <v>1053</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="53"/>
+      <c r="I12" s="55"/>
       <c r="J12" s="31" t="s">
         <v>1052</v>
       </c>
@@ -5756,7 +5762,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="34.5" customHeight="1" thickBot="1">
-      <c r="A13" s="53"/>
+      <c r="A13" s="55"/>
       <c r="B13" s="33" t="s">
         <v>1054</v>
       </c>
@@ -5764,7 +5770,7 @@
         <v>1055</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="53"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="33" t="s">
         <v>1054</v>
       </c>
@@ -5772,7 +5778,7 @@
         <v>1055</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="53"/>
+      <c r="I13" s="55"/>
       <c r="J13" s="33" t="s">
         <v>1054</v>
       </c>
@@ -5781,7 +5787,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="132.75" customHeight="1" thickBot="1">
-      <c r="A14" s="53"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="29" t="s">
         <v>29</v>
       </c>
@@ -5789,7 +5795,7 @@
         <v>1067</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="53"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="29" t="s">
         <v>29</v>
       </c>
@@ -5797,7 +5803,7 @@
         <v>1067</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="53"/>
+      <c r="I14" s="55"/>
       <c r="J14" s="29" t="s">
         <v>29</v>
       </c>
@@ -5806,7 +5812,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="54" customHeight="1" thickBot="1">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="55" t="s">
         <v>1056</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -5816,7 +5822,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="55" t="s">
         <v>1056</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -5826,7 +5832,7 @@
         <v>33</v>
       </c>
       <c r="H15" s="17"/>
-      <c r="I15" s="53" t="s">
+      <c r="I15" s="55" t="s">
         <v>1056</v>
       </c>
       <c r="J15" s="28" t="s">
@@ -5837,7 +5843,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="68.25" customHeight="1" thickBot="1">
-      <c r="A16" s="53"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="31" t="s">
         <v>35</v>
       </c>
@@ -5845,7 +5851,7 @@
         <v>1057</v>
       </c>
       <c r="D16" s="17"/>
-      <c r="E16" s="53"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="31" t="s">
         <v>36</v>
       </c>
@@ -5853,7 +5859,7 @@
         <v>1058</v>
       </c>
       <c r="H16" s="17"/>
-      <c r="I16" s="53"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="31" t="s">
         <v>37</v>
       </c>
@@ -5862,7 +5868,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="84" customHeight="1" thickBot="1">
-      <c r="A17" s="53"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="33" t="s">
         <v>38</v>
       </c>
@@ -5870,7 +5876,7 @@
         <v>39</v>
       </c>
       <c r="D17" s="17"/>
-      <c r="E17" s="53"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="33" t="s">
         <v>38</v>
       </c>
@@ -5878,7 +5884,7 @@
         <v>40</v>
       </c>
       <c r="H17" s="17"/>
-      <c r="I17" s="53"/>
+      <c r="I17" s="55"/>
       <c r="J17" s="33" t="s">
         <v>38</v>
       </c>
@@ -5887,7 +5893,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A18" s="53"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="37" t="s">
         <v>1038</v>
       </c>
@@ -5895,7 +5901,7 @@
         <v>1066</v>
       </c>
       <c r="D18" s="17"/>
-      <c r="E18" s="53"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="37" t="s">
         <v>42</v>
       </c>
@@ -5903,7 +5909,7 @@
         <v>1039</v>
       </c>
       <c r="H18" s="17"/>
-      <c r="I18" s="53"/>
+      <c r="I18" s="55"/>
       <c r="J18" s="37" t="s">
         <v>42</v>
       </c>
@@ -5912,7 +5918,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A19" s="53"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="33" t="s">
         <v>327</v>
       </c>
@@ -5920,7 +5926,7 @@
         <v>1059</v>
       </c>
       <c r="D19" s="17"/>
-      <c r="E19" s="53"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="33" t="s">
         <v>327</v>
       </c>
@@ -5928,7 +5934,7 @@
         <v>1059</v>
       </c>
       <c r="H19" s="17"/>
-      <c r="I19" s="53"/>
+      <c r="I19" s="55"/>
       <c r="J19" s="33" t="s">
         <v>327</v>
       </c>
@@ -5937,7 +5943,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A20" s="53"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="29" t="s">
         <v>328</v>
       </c>
@@ -5945,7 +5951,7 @@
         <v>1061</v>
       </c>
       <c r="D20" s="17"/>
-      <c r="E20" s="53"/>
+      <c r="E20" s="55"/>
       <c r="F20" s="29" t="s">
         <v>328</v>
       </c>
@@ -5953,7 +5959,7 @@
         <v>1062</v>
       </c>
       <c r="H20" s="17"/>
-      <c r="I20" s="53"/>
+      <c r="I20" s="55"/>
       <c r="J20" s="29" t="s">
         <v>328</v>
       </c>
@@ -6051,18 +6057,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="E5:E14"/>
+    <mergeCell ref="I5:I14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="I15:I20"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="E5:E14"/>
-    <mergeCell ref="I5:I14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="I15:I20"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11567,7 +11573,7 @@
         <v>89</v>
       </c>
       <c r="S18" s="16" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="V18"/>
       <c r="W18"/>
@@ -11625,10 +11631,10 @@
         <v>79</v>
       </c>
       <c r="R19" s="16" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="S19" s="16" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="V19"/>
       <c r="W19"/>
@@ -14566,7 +14572,7 @@
   <dimension ref="A1:AR122"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" sqref="A1:B1"/>
@@ -16635,7 +16641,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="16" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="T32"/>
       <c r="AA32"/>
@@ -16701,7 +16707,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="16" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="T33"/>
       <c r="AA33"/>
@@ -16767,7 +16773,7 @@
         <v>1</v>
       </c>
       <c r="S34" s="16" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="T34"/>
       <c r="AA34"/>
@@ -17565,7 +17571,7 @@
         <v>1085</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="P46" s="16" t="s">
         <v>75</v>
@@ -18229,7 +18235,7 @@
         <v>742</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="P56" s="16" t="s">
         <v>68</v>
@@ -18703,7 +18709,7 @@
         <v>1</v>
       </c>
       <c r="S63" s="16" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="T63"/>
       <c r="AA63"/>
@@ -20358,7 +20364,7 @@
         <v>1</v>
       </c>
       <c r="S88" s="16" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="T88"/>
       <c r="AA88"/>
@@ -21283,10 +21289,10 @@
         <v>68</v>
       </c>
       <c r="Q102" s="16" t="s">
-        <v>867</v>
+        <v>1140</v>
       </c>
       <c r="R102" s="16" t="s">
-        <v>879</v>
+        <v>1139</v>
       </c>
       <c r="S102" s="16" t="s">
         <v>885</v>
@@ -21941,7 +21947,7 @@
         <v>1090</v>
       </c>
       <c r="S112" t="s">
-        <v>1091</v>
+        <v>1138</v>
       </c>
       <c r="AA112"/>
       <c r="AB112"/>
@@ -22008,7 +22014,7 @@
         <v>89</v>
       </c>
       <c r="S113" s="16" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="AA113"/>
       <c r="AB113"/>
@@ -22663,7 +22669,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="55" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -22674,7 +22680,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A4" s="53"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="29" t="s">
         <v>161</v>
       </c>
@@ -22808,21 +22814,21 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="51" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="51" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="51" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="5"/>
@@ -27396,7 +27402,7 @@
         <v>301</v>
       </c>
       <c r="E120" s="20" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F120" s="20" t="s">
         <v>60</v>
@@ -27832,7 +27838,7 @@
         <v>69</v>
       </c>
       <c r="E137" s="20" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F137" s="20" t="s">
         <v>61</v>
@@ -28364,7 +28370,7 @@
         <v>291</v>
       </c>
       <c r="E159" s="20" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F159" s="24" t="s">
         <v>60</v>
@@ -28388,7 +28394,7 @@
         <v>191</v>
       </c>
       <c r="E160" s="20" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F160" s="24" t="s">
         <v>60</v>
@@ -28441,7 +28447,7 @@
         <v>283</v>
       </c>
       <c r="E161" s="20" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F161" s="24" t="s">
         <v>60</v>
@@ -28494,7 +28500,7 @@
         <v>192</v>
       </c>
       <c r="E162" s="20" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="F162" s="24" t="s">
         <v>60</v>
@@ -28547,7 +28553,7 @@
         <v>308</v>
       </c>
       <c r="E163" s="20" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F163" s="24" t="s">
         <v>60</v>
@@ -28600,7 +28606,7 @@
         <v>154</v>
       </c>
       <c r="E164" s="20" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F164" s="24" t="s">
         <v>60</v>
@@ -28624,7 +28630,7 @@
         <v>155</v>
       </c>
       <c r="E165" s="20" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F165" s="24" t="s">
         <v>60</v>
@@ -28648,7 +28654,7 @@
         <v>193</v>
       </c>
       <c r="E166" s="20" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="F166" s="24" t="s">
         <v>60</v>
@@ -28672,7 +28678,7 @@
         <v>194</v>
       </c>
       <c r="E167" s="20" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F167" s="24" t="s">
         <v>60</v>
@@ -28696,7 +28702,7 @@
         <v>195</v>
       </c>
       <c r="E168" s="20" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="F168" s="24" t="s">
         <v>60</v>
@@ -28720,7 +28726,7 @@
         <v>196</v>
       </c>
       <c r="E169" s="20" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F169" s="24" t="s">
         <v>60</v>
@@ -28744,7 +28750,7 @@
         <v>156</v>
       </c>
       <c r="E170" s="20" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="F170" s="24" t="s">
         <v>60</v>
@@ -32574,7 +32580,7 @@
         <v>571</v>
       </c>
       <c r="E327" s="20" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F327" s="24" t="s">
         <v>60</v>
@@ -33222,7 +33228,7 @@
         <v>572</v>
       </c>
       <c r="E353" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F353" s="24" t="s">
         <v>314</v>
@@ -33448,7 +33454,7 @@
         <v>574</v>
       </c>
       <c r="E362" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F362" s="24" t="s">
         <v>59</v>
@@ -33664,7 +33670,7 @@
         <v>576</v>
       </c>
       <c r="E371" s="20" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F371" s="24" t="s">
         <v>59</v>
@@ -33884,7 +33890,7 @@
         <v>572</v>
       </c>
       <c r="E380" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F380" s="24" t="s">
         <v>314</v>
@@ -34110,7 +34116,7 @@
         <v>574</v>
       </c>
       <c r="E389" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F389" s="24" t="s">
         <v>59</v>
@@ -34326,7 +34332,7 @@
         <v>576</v>
       </c>
       <c r="E398" s="20" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="F398" s="24" t="s">
         <v>59</v>
@@ -36287,10 +36293,10 @@
         <v>190</v>
       </c>
       <c r="D479" s="20" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E479" s="20" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="F479" s="24" t="s">
         <v>60</v>
@@ -36959,10 +36965,10 @@
         <v>190</v>
       </c>
       <c r="D507" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E507" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F507" s="24" t="s">
         <v>60</v>
@@ -36983,10 +36989,10 @@
         <v>190</v>
       </c>
       <c r="D508" s="20" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E508" s="20" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F508" s="24" t="s">
         <v>60</v>
@@ -37055,10 +37061,10 @@
         <v>190</v>
       </c>
       <c r="D511" s="20" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E511" s="20" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F511" s="24" t="s">
         <v>60</v>
@@ -37103,10 +37109,10 @@
         <v>190</v>
       </c>
       <c r="D513" s="20" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E513" s="20" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F513" s="24" t="s">
         <v>60</v>
@@ -37151,10 +37157,10 @@
         <v>190</v>
       </c>
       <c r="D515" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E515" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F515" s="24" t="s">
         <v>60</v>
@@ -37199,10 +37205,10 @@
         <v>218</v>
       </c>
       <c r="D517" s="20" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E517" s="20" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="F517" s="24" t="s">
         <v>60</v>
@@ -37871,10 +37877,10 @@
         <v>218</v>
       </c>
       <c r="D545" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E545" s="20" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F545" s="24" t="s">
         <v>60</v>
@@ -37895,10 +37901,10 @@
         <v>218</v>
       </c>
       <c r="D546" s="20" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E546" s="20" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="F546" s="24" t="s">
         <v>60</v>
@@ -37967,10 +37973,10 @@
         <v>218</v>
       </c>
       <c r="D549" s="20" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E549" s="20" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="F549" s="24" t="s">
         <v>60</v>
@@ -38015,10 +38021,10 @@
         <v>218</v>
       </c>
       <c r="D551" s="20" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E551" s="20" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F551" s="24" t="s">
         <v>60</v>
@@ -38063,10 +38069,10 @@
         <v>218</v>
       </c>
       <c r="D553" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E553" s="20" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F553" s="24" t="s">
         <v>60</v>
@@ -39122,7 +39128,7 @@
         <v>421</v>
       </c>
       <c r="E597" s="20" t="s">
-        <v>867</v>
+        <v>1140</v>
       </c>
       <c r="F597" s="24" t="s">
         <v>61</v>
@@ -39699,10 +39705,10 @@
         <v>218</v>
       </c>
       <c r="D621" s="20" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E621" s="20" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F621" s="24" t="s">
         <v>60</v>
@@ -40525,7 +40531,7 @@
         <v>291</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>188</v>
@@ -40551,7 +40557,7 @@
         <v>191</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>188</v>
@@ -40577,7 +40583,7 @@
         <v>319</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G5" s="24" t="s">
         <v>188</v>
@@ -40603,7 +40609,7 @@
         <v>321</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>318</v>
@@ -40620,16 +40626,16 @@
         <v>152</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>317</v>
       </c>
       <c r="H7" s="52" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -40735,10 +40741,10 @@
         <v>218</v>
       </c>
       <c r="D12" s="16" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>1131</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>1132</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>317</v>
@@ -40758,10 +40764,10 @@
         <v>218</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>1133</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>1134</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>317</v>
@@ -40781,10 +40787,10 @@
         <v>218</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>1135</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>1136</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>317</v>
@@ -40804,10 +40810,10 @@
         <v>218</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>1137</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1138</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>317</v>
@@ -40859,6 +40865,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="38934ba0-d0c8-4ff1-b39d-50890708cb62">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058BEFEFAD17A4B43A8378381BF28CF4F" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61556453c3d4cfbe4714da52328c09a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="38934ba0-d0c8-4ff1-b39d-50890708cb62" xmlns:ns3="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xmlns:ns4="ab274330-b409-4ff8-b8ad-c1dc18cc66a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8714ab872510242edcc52d3716bf4cc" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="38934ba0-d0c8-4ff1-b39d-50890708cb62"/>
@@ -41112,17 +41129,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="38934ba0-d0c8-4ff1-b39d-50890708cb62">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AA5E4F3-9B72-420C-85C5-8B45D533C3CA}">
   <ds:schemaRefs>
@@ -41132,6 +41138,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{281A6493-1F0C-453E-819E-2ED93017F2F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38934ba0-d0c8-4ff1-b39d-50890708cb62"/>
+    <ds:schemaRef ds:uri="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42637C87-0D45-4DE4-998D-7915D289D5B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41149,15 +41166,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{281A6493-1F0C-453E-819E-2ED93017F2F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38934ba0-d0c8-4ff1-b39d-50890708cb62"/>
-    <ds:schemaRef ds:uri="ab06a5aa-8e31-4bdb-9b13-38c58a92ec8a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>